<commit_message>
First draft for CIVE 596
</commit_message>
<xml_diff>
--- a/Data/Q/Cross_Section_Surveys/N2_cross_section.xlsx
+++ b/Data/Q/Cross_Section_Surveys/N2_cross_section.xlsx
@@ -15,9 +15,6 @@
     <sheet name="N2-1" sheetId="1" r:id="rId1"/>
     <sheet name="N2-1_m" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -204,27 +201,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -464,11 +441,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="502550944"/>
-        <c:axId val="519349016"/>
+        <c:axId val="277534416"/>
+        <c:axId val="277531280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="502550944"/>
+        <c:axId val="277534416"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="18"/>
@@ -506,12 +483,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519349016"/>
+        <c:crossAx val="277531280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="519349016"/>
+        <c:axId val="277531280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,21 +511,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="502550944"/>
+        <c:crossAx val="277534416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -726,7 +701,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>-1.3525499999999999</c:v>
+                  <c:v>-0.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-1.3525499999999999</c:v>
@@ -771,7 +746,7 @@
                   <c:v>-1.7462499999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.7462499999999999</c:v>
+                  <c:v>-0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -786,11 +761,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="506705328"/>
-        <c:axId val="506708072"/>
+        <c:axId val="333907208"/>
+        <c:axId val="333909560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="506705328"/>
+        <c:axId val="333907208"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="18"/>
@@ -828,12 +803,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="506708072"/>
+        <c:crossAx val="333909560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="506708072"/>
+        <c:axId val="333909560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,7 +838,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="506705328"/>
+        <c:crossAx val="333907208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -964,166 +939,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="N1-1"/>
-      <sheetName val="N1-2"/>
-      <sheetName val="N1-3"/>
-      <sheetName val="N2-1"/>
-      <sheetName val="N2-2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="4">
-          <cell r="H4" t="str">
-            <v>Depth</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="H5" t="str">
-            <v>cm</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>1.66</v>
-          </cell>
-          <cell r="H6">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>1.66</v>
-          </cell>
-          <cell r="H7">
-            <v>-135.255</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>1.833</v>
-          </cell>
-          <cell r="H8">
-            <v>-178.435</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>3</v>
-          </cell>
-          <cell r="H9">
-            <v>-180.97499999999999</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>4</v>
-          </cell>
-          <cell r="H10">
-            <v>-184.15</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>5</v>
-          </cell>
-          <cell r="H11">
-            <v>-177.16499999999999</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>6</v>
-          </cell>
-          <cell r="H12">
-            <v>-180.34</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>7</v>
-          </cell>
-          <cell r="H13">
-            <v>-180.97499999999999</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>8</v>
-          </cell>
-          <cell r="H14">
-            <v>-180.97499999999999</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>9</v>
-          </cell>
-          <cell r="H15">
-            <v>-185.42000000000002</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>10</v>
-          </cell>
-          <cell r="H16">
-            <v>-152.4</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>11</v>
-          </cell>
-          <cell r="H17">
-            <v>-176.53</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>12</v>
-          </cell>
-          <cell r="H18">
-            <v>-174.625</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>13</v>
-          </cell>
-          <cell r="H19">
-            <v>-181.61</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>14.833</v>
-          </cell>
-          <cell r="H20">
-            <v>-174.625</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>14.833</v>
-          </cell>
-          <cell r="H21">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1849,7 +1664,7 @@
   <dimension ref="A2:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,7 +1770,7 @@
       </c>
       <c r="R5">
         <f>SUM(Q6:Q26)</f>
-        <v>4.7736386515970297</v>
+        <v>6.2198886515970297</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1978,12 +1793,11 @@
         <v>1.3525499999999999</v>
       </c>
       <c r="H6" s="14">
-        <f>-G6</f>
-        <v>-1.3525499999999999</v>
+        <v>-0.3</v>
       </c>
       <c r="I6" s="15">
         <f>H6+MAX($G$6:$G$26)</f>
-        <v>0.50164999999999993</v>
+        <v>1.5541999999999998</v>
       </c>
       <c r="J6">
         <f>0</f>
@@ -1996,11 +1810,11 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15">
         <f>$L$4-I6</f>
-        <v>-0.48164999999999991</v>
+        <v>-1.5341999999999998</v>
       </c>
       <c r="N6">
         <f>K6*(L6+M6)*0.5</f>
-        <v>-0.12184974359999998</v>
+        <v>-0.3881280527999999</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2043,7 +1857,7 @@
       </c>
       <c r="L7" s="15">
         <f>M6</f>
-        <v>-0.48164999999999991</v>
+        <v>-1.5341999999999998</v>
       </c>
       <c r="M7" s="15">
         <f>$L$4-I7</f>
@@ -2703,7 +2517,7 @@
         <v>1.7462499999999999</v>
       </c>
       <c r="H20" s="14">
-        <f t="shared" ref="H20:H21" si="12">-G20</f>
+        <f t="shared" ref="H20" si="12">-G20</f>
         <v>-1.7462499999999999</v>
       </c>
       <c r="I20" s="15">
@@ -2755,12 +2569,11 @@
         <v>1.7462499999999999</v>
       </c>
       <c r="H21" s="14">
-        <f t="shared" si="12"/>
-        <v>-1.7462499999999999</v>
+        <v>-0.3</v>
       </c>
       <c r="I21" s="15">
         <f t="shared" si="13"/>
-        <v>0.10794999999999999</v>
+        <v>1.5541999999999998</v>
       </c>
       <c r="J21" s="15">
         <f t="shared" si="14"/>
@@ -2776,7 +2589,7 @@
       </c>
       <c r="M21" s="15">
         <f t="shared" si="17"/>
-        <v>-8.7949999999999987E-2</v>
+        <v>-1.5341999999999998</v>
       </c>
       <c r="N21">
         <f t="shared" si="18"/>
@@ -2784,7 +2597,7 @@
       </c>
       <c r="Q21" s="15">
         <f t="shared" si="19"/>
-        <v>8.7949999999999987E-2</v>
+        <v>1.5341999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -2797,7 +2610,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L6:M21">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>